<commit_message>
Agregando una tabla adicional a requerimiento
</commit_message>
<xml_diff>
--- a/ENMASCARARMANTTABLAS.xlsx
+++ b/ENMASCARARMANTTABLAS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2596" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="871">
   <si>
     <t>OWNER</t>
   </si>
@@ -2637,13 +2637,16 @@
   </si>
   <si>
     <t>PRESTAMOCUOTASFECHA</t>
+  </si>
+  <si>
+    <t>CUENTACORRIENTEACTIVA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2661,6 +2664,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2683,10 +2694,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2967,7 +2979,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D865"/>
+  <dimension ref="A1:D866"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2979,7 +2991,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -12493,6 +12505,17 @@
         <v>862</v>
       </c>
       <c r="C865" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="866" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A866" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B866" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="C866" t="s">
         <v>863</v>
       </c>
     </row>
@@ -12504,5 +12527,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>